<commit_message>
Neural Network with very bad learning rate
</commit_message>
<xml_diff>
--- a/Experimental/Workflow.xlsx
+++ b/Experimental/Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\Space-Platypus\Experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF3683-D256-4C8C-A689-C6D93F826EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED47E4DD-AA33-4818-9D33-071048EEF982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15225" yWindow="2625" windowWidth="32565" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>STA/LTA</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>End time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal </t>
+  </si>
+  <si>
+    <t>Frequencies</t>
+  </si>
+  <si>
+    <t>Power/Amplitude</t>
+  </si>
+  <si>
+    <t>Frequency intervals</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,82 +416,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:H9"/>
+  <dimension ref="A4:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="G5" s="2" t="s">
+      <c r="F7" s="3"/>
+      <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="I7" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="D5:E5"/>
+  <mergeCells count="3">
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Kept only NN Module test 2 and functions
</commit_message>
<xml_diff>
--- a/Experimental/Workflow.xlsx
+++ b/Experimental/Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\Space-Platypus\Experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD464D3-315D-4C23-B19C-D6426DA81B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50067F64-953F-4997-AADB-A9505BD70FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="25980" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18015" yWindow="1890" windowWidth="29655" windowHeight="18885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>STA/LTA</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Noise</t>
   </si>
   <si>
-    <t>Will</t>
-  </si>
-  <si>
     <t>Jeff</t>
   </si>
   <si>
@@ -120,6 +117,18 @@
   </si>
   <si>
     <t>General Region</t>
+  </si>
+  <si>
+    <t>Will/Laurance</t>
+  </si>
+  <si>
+    <t>Transfer learning</t>
+  </si>
+  <si>
+    <t>To look into</t>
+  </si>
+  <si>
+    <t>filtering and use of Classical methods</t>
   </si>
 </sst>
 </file>
@@ -163,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -177,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +761,7 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -777,11 +789,11 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
@@ -815,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -847,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" t="s">
         <v>16</v>
@@ -861,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H11" s="2"/>
       <c r="K11" t="s">
@@ -903,13 +915,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
       <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
@@ -917,7 +942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>6</v>
       </c>
@@ -925,23 +950,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>